<commit_message>
Reordered in order of difficulty.
</commit_message>
<xml_diff>
--- a/Day3/SNV_filtering_practical.xlsx
+++ b/Day3/SNV_filtering_practical.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>Chromosome</t>
   </si>
@@ -530,7 +530,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -598,16 +598,16 @@
     </row>
     <row r="3" spans="1:8" ht="45">
       <c r="A3" s="1">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1">
-        <v>38120429</v>
+        <v>106471685</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E3" s="4" t="str">
         <f>HYPERLINK("http://localhost:60151/goto?locus="&amp;A3&amp;":"&amp;B3, "IGV")</f>
@@ -617,24 +617,24 @@
         <v>0</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30">
       <c r="A4" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
-        <v>106471685</v>
+        <v>91537757</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="E4" s="4" t="str">
         <f>HYPERLINK("http://localhost:60151/goto?locus="&amp;A4&amp;":"&amp;B4, "IGV")</f>
@@ -644,48 +644,48 @@
         <v>0</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="45">
       <c r="A5" s="1">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1">
-        <v>9633452</v>
+        <v>38120429</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E5" s="4" t="str">
         <f>HYPERLINK("http://localhost:60151/goto?locus="&amp;A5&amp;":"&amp;B5, "IGV")</f>
         <v>IGV</v>
       </c>
-      <c r="F5" s="2" t="b">
-        <v>1</v>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30">
+        <v>16</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45">
       <c r="A6" s="1">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1">
-        <v>91537757</v>
+        <v>9983580</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="E6" s="4" t="str">
         <f>HYPERLINK("http://localhost:60151/goto?locus="&amp;A6&amp;":"&amp;B6, "IGV")</f>
@@ -695,39 +695,39 @@
         <v>0</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="75">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30">
       <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>9633452</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4" t="str">
+        <f>HYPERLINK("http://localhost:60151/goto?locus="&amp;A7&amp;":"&amp;B7, "IGV")</f>
+        <v>IGV</v>
+      </c>
+      <c r="F7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="75">
+      <c r="A8" s="1">
         <v>3</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B8" s="1">
         <v>177090982</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="4" t="str">
-        <f t="shared" ref="E7:E11" si="0">HYPERLINK("http://localhost:60151/goto?locus="&amp;A7&amp;":"&amp;B7, "IGV")</f>
-        <v>IGV</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="1">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1">
-        <v>68175783</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>10</v>
@@ -736,52 +736,52 @@
         <v>9</v>
       </c>
       <c r="E8" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>IGV</v>
-      </c>
-      <c r="F8" s="2" t="b">
-        <v>0</v>
+        <f t="shared" ref="E8:E11" si="0">HYPERLINK("http://localhost:60151/goto?locus="&amp;A8&amp;":"&amp;B8, "IGV")</f>
+        <v>IGV</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="30">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1">
-        <v>140281877</v>
+        <v>68175783</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>IGV</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>12</v>
+      <c r="F9" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="45">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30">
       <c r="A10" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B10" s="1">
-        <v>9983580</v>
+        <v>140281877</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>5</v>
@@ -790,11 +790,11 @@
         <f t="shared" si="0"/>
         <v>IGV</v>
       </c>
-      <c r="F10" s="2" t="b">
-        <v>0</v>
+      <c r="F10" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="45">

</xml_diff>